<commit_message>
endpoint /tags/[id]/quiz côté back OK"
</commit_message>
<xml_diff>
--- a/backend/docs/routes.xlsx
+++ b/backend/docs/routes.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuille 1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Stories" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Routes" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,145 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="96">
+  <si>
+    <t xml:space="preserve">En tant que...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai besoin de...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">afin de...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difficulté/Durée (1à5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commentaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Back</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Front</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visiteur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">une page d'accueil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prévisualiser le contenu du site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">première route, page d'accueil avec les quiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visualiser les titres de quiz sur la page d’accueil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choisir le quiz que je souhaite effectuer et y accéder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir accéder aux questions d’un quiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir visualiser la difficulté de chaque question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accéder à un formulaire d’inscription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir m’inscrire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accéder à un formulaire de connexion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir me connecter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avoir un compte et répondre aux quiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir me connecter à mon compte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir répondre aux quiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">membre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir accéder à ma page profil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visualiser les données de mon compte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir répondre aux questions d’un quiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vérifier mes connaissances</t>
+  </si>
+  <si>
+    <t xml:space="preserve">même page d’un quiz, mais avec la possibilité de choisir les réponses pour les soumettre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir visualiser mon score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir visualiser les bonnes et mauvaise réponses que j’ai donné</t>
+  </si>
+  <si>
+    <t xml:space="preserve">savoir quelles erreurs j’ai effectué</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir me déconnecter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visualiser les sujets de chaque quiz sur la page du quiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir visualiser tous les sujets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">afin de pouvoir accéder aux quiz d’un sujet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir visualiser tous les quiz pour un sujet donné</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avoir un espace admin réservé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir gérer le contenu du site de quiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir ajouter/modifier/supprimer un sujet/tag de quiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir modifier les données de chaque quiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir modifier les données de chaque question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir recevoir par email un résumé du quiz et de mes réponses pour chaque participation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">garder une trace des quiz auxquels j’ai participé</t>
+  </si>
   <si>
     <t xml:space="preserve">URL</t>
   </si>
@@ -59,6 +198,9 @@
   </si>
   <si>
     <t xml:space="preserve">home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Back OK</t>
   </si>
   <si>
     <t xml:space="preserve">/quiz/[id]</t>
@@ -176,12 +318,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -200,27 +342,39 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="12"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="14"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,8 +383,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFEFEFEF"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
   </fills>
@@ -275,16 +435,36 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -292,11 +472,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -316,7 +496,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFEFEFEF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -381,299 +561,665 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:H65536"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.6377551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.2397959183674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.1479591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="56.1581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="8.96428571428571"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AB65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="70.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="47.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="14.43"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="71.6734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="46.8418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="14.1734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="25.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
+    <row r="1" s="8" customFormat="true" ht="25.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="9"/>
+      <c r="AB2" s="9"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>17</v>
+        <v>64</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>13</v>
+      <c r="A4" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>38</v>
+        <v>85</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>39</v>
+        <v>86</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>40</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>43</v>
+        <v>90</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>44</v>
+        <v>91</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>47</v>
+        <v>94</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>48</v>
+        <v>95</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -712,7 +1258,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
endpoint /tags/[id]/quiz côté back OK
</commit_message>
<xml_diff>
--- a/backend/docs/routes.xlsx
+++ b/backend/docs/routes.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuille 1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Stories" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Routes" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,145 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="96">
+  <si>
+    <t xml:space="preserve">En tant que...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai besoin de...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">afin de...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difficulté/Durée (1à5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commentaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Back</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Front</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visiteur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">une page d'accueil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prévisualiser le contenu du site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">première route, page d'accueil avec les quiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visualiser les titres de quiz sur la page d’accueil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choisir le quiz que je souhaite effectuer et y accéder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir accéder aux questions d’un quiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir visualiser la difficulté de chaque question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accéder à un formulaire d’inscription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir m’inscrire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accéder à un formulaire de connexion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir me connecter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avoir un compte et répondre aux quiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir me connecter à mon compte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir répondre aux quiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">membre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir accéder à ma page profil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visualiser les données de mon compte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir répondre aux questions d’un quiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vérifier mes connaissances</t>
+  </si>
+  <si>
+    <t xml:space="preserve">même page d’un quiz, mais avec la possibilité de choisir les réponses pour les soumettre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir visualiser mon score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir visualiser les bonnes et mauvaise réponses que j’ai donné</t>
+  </si>
+  <si>
+    <t xml:space="preserve">savoir quelles erreurs j’ai effectué</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir me déconnecter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visualiser les sujets de chaque quiz sur la page du quiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir visualiser tous les sujets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">afin de pouvoir accéder aux quiz d’un sujet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir visualiser tous les quiz pour un sujet donné</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avoir un espace admin réservé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir gérer le contenu du site de quiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir ajouter/modifier/supprimer un sujet/tag de quiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir modifier les données de chaque quiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir modifier les données de chaque question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir recevoir par email un résumé du quiz et de mes réponses pour chaque participation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">garder une trace des quiz auxquels j’ai participé</t>
+  </si>
   <si>
     <t xml:space="preserve">URL</t>
   </si>
@@ -59,6 +198,9 @@
   </si>
   <si>
     <t xml:space="preserve">home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Back OK</t>
   </si>
   <si>
     <t xml:space="preserve">/quiz/[id]</t>
@@ -176,12 +318,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -200,27 +342,39 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="12"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="14"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,8 +383,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFEFEFEF"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
   </fills>
@@ -275,16 +435,36 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -292,11 +472,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -316,7 +496,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFEFEFEF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -381,299 +561,665 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:H65536"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.6377551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.2397959183674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.1479591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="56.1581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="8.96428571428571"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AB65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="70.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="47.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="14.43"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="71.6734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="46.8418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="14.1734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="25.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
+    <row r="1" s="8" customFormat="true" ht="25.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="9"/>
+      <c r="AB2" s="9"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>17</v>
+        <v>64</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>13</v>
+      <c r="A4" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>38</v>
+        <v>85</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>39</v>
+        <v>86</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>40</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>43</v>
+        <v>90</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>44</v>
+        <v>91</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>47</v>
+        <v>94</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>48</v>
+        <v>95</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -712,7 +1258,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>